<commit_message>
parser clean up , xlsx documentation and generation
</commit_message>
<xml_diff>
--- a/Documentation/bydtatype.xlsx
+++ b/Documentation/bydtatype.xlsx
@@ -921,8 +921,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ97"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J89" activeCellId="0" sqref="J89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -931,12 +931,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="63.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="29.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="34.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="8.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="5.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.66"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.52"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
New version with auto gen code
</commit_message>
<xml_diff>
--- a/Documentation/bydtatype.xlsx
+++ b/Documentation/bydtatype.xlsx
@@ -392,11 +392,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -415,136 +416,18 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF0000EE"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFE0EFD4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFE0EFD4"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -555,11 +438,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE0EFD4"/>
-        <bgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -567,23 +450,8 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -607,57 +475,6 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -680,15 +497,15 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -696,50 +513,33 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000EE"/>
+      <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
@@ -747,11 +547,11 @@
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFE0EFD4"/>
+      <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -762,12 +562,12 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFE0EFD4"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -800,8 +600,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ94"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>